<commit_message>
Modification du fichier de config Configcategorie.xlsx pour rajouter des expéditeurs
</commit_message>
<xml_diff>
--- a/Data/ConfigCategorie.xlsx
+++ b/Data/ConfigCategorie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlemoallic\Documents\UiPath\TriageMail\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E59002-60B4-462C-BF6C-F652FE7346F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EF470B-A186-4ABD-A25C-D705C9AD81E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TEXTILE</t>
   </si>
@@ -63,10 +63,13 @@
     <t>BZB;wish;Jules</t>
   </si>
   <si>
-    <t>Easy cash;Call of duty;Nintendo;Instant gaming;leboncoin;fnac;figurines</t>
-  </si>
-  <si>
     <t>MAAF;bouygues</t>
+  </si>
+  <si>
+    <t>AUTRE</t>
+  </si>
+  <si>
+    <t>Easy cash;Call of duty;Nintendo;Instant gaming;leboncoin;fnac;figurines;micromania</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -448,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -464,6 +467,11 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changement du redimenssionement de la page gmail à l'ouverture
</commit_message>
<xml_diff>
--- a/Data/ConfigCategorie.xlsx
+++ b/Data/ConfigCategorie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlemoallic\Documents\UiPath\TriageMail\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EF470B-A186-4ABD-A25C-D705C9AD81E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C1BD74-DB44-4CFE-A140-E1C7C0C46095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Talent.com;HelloWork;Jungle;Linkedin;capgemini;emploi;meteojob</t>
-  </si>
-  <si>
     <t>ASSURANCE</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Easy cash;Call of duty;Nintendo;Instant gaming;leboncoin;fnac;figurines;micromania</t>
+  </si>
+  <si>
+    <t>Talent.com;HelloWork;Jungle;Linkedin;capgemini;emploi;meteojob;mission-locale</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -438,12 +438,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -451,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -464,15 +464,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>